<commit_message>
remove redundant codes in biogenic refinery
</commit_message>
<xml_diff>
--- a/exposan/biogenic_refinery/results/uncertaintyD.xlsx
+++ b/exposan/biogenic_refinery/results/uncertaintyD.xlsx
@@ -2892,16 +2892,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>12.93363662479974</v>
+        <v>53.07492191862304</v>
       </c>
       <c r="C4" t="n">
-        <v>8.75763766355489</v>
+        <v>40.60040820824047</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>4.175998961244851</v>
+        <v>12.47451371038257</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -2910,19 +2910,19 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>72.87539832236907</v>
+        <v>120.8425334270357</v>
       </c>
       <c r="I4" t="n">
-        <v>23.68856774874473</v>
+        <v>70.09140696976552</v>
       </c>
       <c r="J4" t="n">
-        <v>0.338927913791387</v>
+        <v>0.4777504782706036</v>
       </c>
       <c r="K4" t="n">
-        <v>48.84790265983295</v>
+        <v>50.27337597899956</v>
       </c>
       <c r="L4" t="n">
-        <v>-7.105427357601002e-15</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -3159,16 +3159,16 @@
         <v>0</v>
       </c>
       <c r="CM4" t="n">
-        <v>0.02476305948249567</v>
+        <v>0.1148015437608499</v>
       </c>
       <c r="CN4" t="n">
-        <v>0.005579691985774974</v>
+        <v>0.02586745204605278</v>
       </c>
       <c r="CO4" t="n">
         <v>0</v>
       </c>
       <c r="CP4" t="n">
-        <v>0.005861401058731467</v>
+        <v>0.008309297845406316</v>
       </c>
       <c r="CQ4" t="n">
         <v>0</v>
@@ -3234,7 +3234,7 @@
         <v>0</v>
       </c>
       <c r="DL4" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM4" t="n">
         <v>0</v>
@@ -3243,13 +3243,13 @@
         <v>0</v>
       </c>
       <c r="DO4" t="n">
-        <v>31.31172703820987</v>
+        <v>32.20646951438269</v>
       </c>
       <c r="DP4" t="n">
-        <v>0.338927913791387</v>
+        <v>0.4777504782706036</v>
       </c>
       <c r="DQ4" t="n">
-        <v>0.07174037415993204</v>
+        <v>0.07226864719535553</v>
       </c>
       <c r="DR4" t="n">
         <v>0</v>
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="DT4" t="n">
-        <v>17.30365112364506</v>
+        <v>17.80860408288861</v>
       </c>
       <c r="DU4" t="n">
         <v>0</v>
@@ -3338,16 +3338,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>12.60825199473375</v>
+        <v>52.53864100310895</v>
       </c>
       <c r="C5" t="n">
-        <v>8.046637077697969</v>
+        <v>37.30420949220779</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>4.561614917035778</v>
+        <v>15.23443151090117</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -3356,19 +3356,19 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>74.02453503439295</v>
+        <v>121.8121045053803</v>
       </c>
       <c r="I5" t="n">
-        <v>22.99206310585224</v>
+        <v>69.21498657186895</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1982666100919121</v>
+        <v>0.2794752628572355</v>
       </c>
       <c r="K5" t="n">
-        <v>50.8342053184488</v>
+        <v>52.31764267065415</v>
       </c>
       <c r="L5" t="n">
-        <v>7.105427357601002e-15</v>
+        <v>-1.4210854715202e-14</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -3605,16 +3605,16 @@
         <v>0</v>
       </c>
       <c r="CM5" t="n">
-        <v>0.02275263721155219</v>
+        <v>0.105481226112756</v>
       </c>
       <c r="CN5" t="n">
-        <v>0.007463787951843422</v>
+        <v>0.0346021209447461</v>
       </c>
       <c r="CO5" t="n">
         <v>0</v>
       </c>
       <c r="CP5" t="n">
-        <v>0.005033787163323094</v>
+        <v>0.007136047578270794</v>
       </c>
       <c r="CQ5" t="n">
         <v>0</v>
@@ -3680,7 +3680,7 @@
         <v>0</v>
       </c>
       <c r="DL5" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM5" t="n">
         <v>0</v>
@@ -3689,13 +3689,13 @@
         <v>0</v>
       </c>
       <c r="DO5" t="n">
-        <v>31.97965694956584</v>
+        <v>32.90304280249227</v>
       </c>
       <c r="DP5" t="n">
-        <v>0.1982666100919121</v>
+        <v>0.2794752628572355</v>
       </c>
       <c r="DQ5" t="n">
-        <v>0.06519719831077456</v>
+        <v>0.06575874043806755</v>
       </c>
       <c r="DR5" t="n">
         <v>0</v>
@@ -3704,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="DT5" t="n">
-        <v>18.48643221991453</v>
+        <v>19.02590094756042</v>
       </c>
       <c r="DU5" t="n">
         <v>0</v>
@@ -3784,16 +3784,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>11.66083194546483</v>
+        <v>47.98375005106177</v>
       </c>
       <c r="C6" t="n">
-        <v>8.285566716434916</v>
+        <v>38.41188729739226</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>3.375265229029914</v>
+        <v>9.57186275366951</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -3802,16 +3802,16 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>62.96274096146484</v>
+        <v>109.3780958480188</v>
       </c>
       <c r="I6" t="n">
-        <v>18.2484411373995</v>
+        <v>63.22885124936731</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3419922752653987</v>
+        <v>0.4820699813278353</v>
       </c>
       <c r="K6" t="n">
-        <v>44.37230754879994</v>
+        <v>45.66717461732365</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -4051,16 +4051,16 @@
         <v>0</v>
       </c>
       <c r="CM6" t="n">
-        <v>0.02342823365473416</v>
+        <v>0.1086132912233476</v>
       </c>
       <c r="CN6" t="n">
-        <v>0.004075053181495331</v>
+        <v>0.01889194654941236</v>
       </c>
       <c r="CO6" t="n">
         <v>0</v>
       </c>
       <c r="CP6" t="n">
-        <v>0.005172248815846901</v>
+        <v>0.007332334967490409</v>
       </c>
       <c r="CQ6" t="n">
         <v>0</v>
@@ -4126,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="DL6" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM6" t="n">
         <v>0</v>
@@ -4135,13 +4135,13 @@
         <v>0</v>
       </c>
       <c r="DO6" t="n">
-        <v>24.73174899418314</v>
+        <v>25.43068093247103</v>
       </c>
       <c r="DP6" t="n">
-        <v>0.3419922752653987</v>
+        <v>0.4820699813278353</v>
       </c>
       <c r="DQ6" t="n">
-        <v>0.1035936374226998</v>
+        <v>0.1039599510111723</v>
       </c>
       <c r="DR6" t="n">
         <v>0</v>
@@ -4150,7 +4150,7 @@
         <v>0</v>
       </c>
       <c r="DT6" t="n">
-        <v>18.84771088906654</v>
+        <v>19.3977224051561</v>
       </c>
       <c r="DU6" t="n">
         <v>0</v>
@@ -4230,16 +4230,16 @@
         <v>3</v>
       </c>
       <c r="B7" t="n">
-        <v>12.16030209936665</v>
+        <v>48.99286447743441</v>
       </c>
       <c r="C7" t="n">
-        <v>7.597101077101502</v>
+        <v>35.22016059344256</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>4.56320102226515</v>
+        <v>13.77270388399185</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -4248,19 +4248,19 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>62.2493383636166</v>
+        <v>109.2717074201711</v>
       </c>
       <c r="I7" t="n">
-        <v>20.8548915018816</v>
+        <v>66.51489193307084</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4058793871632823</v>
+        <v>0.5721248190162059</v>
       </c>
       <c r="K7" t="n">
-        <v>40.98856747457172</v>
+        <v>42.18469066808411</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>-7.105427357601002e-15</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -4497,16 +4497,16 @@
         <v>0</v>
       </c>
       <c r="CM7" t="n">
-        <v>0.02148153110395206</v>
+        <v>0.09958837819792177</v>
       </c>
       <c r="CN7" t="n">
-        <v>0.006217537987600159</v>
+        <v>0.02882450611051433</v>
       </c>
       <c r="CO7" t="n">
         <v>0</v>
       </c>
       <c r="CP7" t="n">
-        <v>0.006284382621345458</v>
+        <v>0.008908929188093469</v>
       </c>
       <c r="CQ7" t="n">
         <v>0</v>
@@ -4572,7 +4572,7 @@
         <v>0</v>
       </c>
       <c r="DL7" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM7" t="n">
         <v>0</v>
@@ -4581,13 +4581,13 @@
         <v>0</v>
       </c>
       <c r="DO7" t="n">
-        <v>20.17327539089239</v>
+        <v>20.72935413002364</v>
       </c>
       <c r="DP7" t="n">
-        <v>0.4058793871632823</v>
+        <v>0.5721248190162059</v>
       </c>
       <c r="DQ7" t="n">
-        <v>0.05869951665293795</v>
+        <v>0.05929409655469964</v>
       </c>
       <c r="DR7" t="n">
         <v>0</v>
@@ -4596,7 +4596,7 @@
         <v>0</v>
       </c>
       <c r="DT7" t="n">
-        <v>19.92535482212201</v>
+        <v>20.50681400721038</v>
       </c>
       <c r="DU7" t="n">
         <v>0</v>
@@ -4676,16 +4676,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>13.34287344983246</v>
+        <v>55.34147991565375</v>
       </c>
       <c r="C8" t="n">
-        <v>8.882346439177008</v>
+        <v>41.17855809202459</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>4.460527010655454</v>
+        <v>14.16292182362916</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -4694,19 +4694,19 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>67.8433678359375</v>
+        <v>115.8178025890695</v>
       </c>
       <c r="I8" t="n">
-        <v>24.46354123910693</v>
+        <v>71.06755766119238</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2747387167451594</v>
+        <v>0.3872698234151387</v>
       </c>
       <c r="K8" t="n">
-        <v>43.10508788008541</v>
+        <v>44.36297510446196</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>-1.4210854715202e-14</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
@@ -4943,16 +4943,16 @@
         <v>0</v>
       </c>
       <c r="CM8" t="n">
-        <v>0.02511568549276911</v>
+        <v>0.1164363179444776</v>
       </c>
       <c r="CN8" t="n">
-        <v>0.006673628384421504</v>
+        <v>0.03093894119017809</v>
       </c>
       <c r="CO8" t="n">
         <v>0</v>
       </c>
       <c r="CP8" t="n">
-        <v>0.005546993562579741</v>
+        <v>0.007863584354011391</v>
       </c>
       <c r="CQ8" t="n">
         <v>0</v>
@@ -5018,7 +5018,7 @@
         <v>0</v>
       </c>
       <c r="DL8" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM8" t="n">
         <v>0</v>
@@ -5027,13 +5027,13 @@
         <v>0</v>
       </c>
       <c r="DO8" t="n">
-        <v>29.49369220214028</v>
+        <v>30.31368469163715</v>
       </c>
       <c r="DP8" t="n">
-        <v>0.2747387167451594</v>
+        <v>0.3872698234151387</v>
       </c>
       <c r="DQ8" t="n">
-        <v>0.09726974309297991</v>
+        <v>0.09766821082590436</v>
       </c>
       <c r="DR8" t="n">
         <v>0</v>
@@ -5042,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="DT8" t="n">
-        <v>13.49435992054572</v>
+        <v>13.88815062554126</v>
       </c>
       <c r="DU8" t="n">
         <v>0</v>
@@ -5122,16 +5122,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="n">
-        <v>11.80149927366452</v>
+        <v>47.48509678100757</v>
       </c>
       <c r="C9" t="n">
-        <v>8.377300894103382</v>
+        <v>38.83716694506329</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>3.424198379561138</v>
+        <v>8.64792983594428</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -5140,19 +5140,19 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>61.59357552985915</v>
+        <v>107.867153854678</v>
       </c>
       <c r="I9" t="n">
-        <v>17.62779247367044</v>
+        <v>62.47247001385377</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3835239835955752</v>
+        <v>0.5406127944475297</v>
       </c>
       <c r="K9" t="n">
-        <v>43.58225907259314</v>
+        <v>44.85407104637666</v>
       </c>
       <c r="L9" t="n">
-        <v>-7.105427357601002e-15</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -5389,16 +5389,16 @@
         <v>0</v>
       </c>
       <c r="CM9" t="n">
-        <v>0.0236876208303004</v>
+        <v>0.1098158101692727</v>
       </c>
       <c r="CN9" t="n">
-        <v>0.003229477509946293</v>
+        <v>0.01497185773611101</v>
       </c>
       <c r="CO9" t="n">
         <v>0</v>
       </c>
       <c r="CP9" t="n">
-        <v>0.00615188791350888</v>
+        <v>0.008721100718530854</v>
       </c>
       <c r="CQ9" t="n">
         <v>0</v>
@@ -5464,7 +5464,7 @@
         <v>0</v>
       </c>
       <c r="DL9" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM9" t="n">
         <v>0</v>
@@ -5473,13 +5473,13 @@
         <v>0</v>
       </c>
       <c r="DO9" t="n">
-        <v>22.67909698300534</v>
+        <v>23.27151744402144</v>
       </c>
       <c r="DP9" t="n">
-        <v>0.3835239835955752</v>
+        <v>0.5406127944475297</v>
       </c>
       <c r="DQ9" t="n">
-        <v>0.04986302666280219</v>
+        <v>0.05050253612232956</v>
       </c>
       <c r="DR9" t="n">
         <v>0</v>
@@ -5488,7 +5488,7 @@
         <v>0</v>
       </c>
       <c r="DT9" t="n">
-        <v>18.85710077491159</v>
+        <v>19.40738630546264</v>
       </c>
       <c r="DU9" t="n">
         <v>0</v>
@@ -5568,16 +5568,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>12.09269637468582</v>
+        <v>49.3886957956508</v>
       </c>
       <c r="C10" t="n">
-        <v>9.102896983728815</v>
+        <v>42.20103041656679</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>2.989799390957009</v>
+        <v>7.187665379084021</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -5586,16 +5586,16 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>67.26908818467135</v>
+        <v>114.6062087949535</v>
       </c>
       <c r="I10" t="n">
-        <v>21.51077123520369</v>
+        <v>67.33756740460419</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4600573509409428</v>
+        <v>0.6484937076596962</v>
       </c>
       <c r="K10" t="n">
-        <v>45.2982595985267</v>
+        <v>46.62014768268961</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
@@ -5835,16 +5835,16 @@
         <v>0</v>
       </c>
       <c r="CM10" t="n">
-        <v>0.02573931328641045</v>
+        <v>0.1193274563957989</v>
       </c>
       <c r="CN10" t="n">
-        <v>0.002510618403415571</v>
+        <v>0.01163922691823459</v>
       </c>
       <c r="CO10" t="n">
         <v>0</v>
       </c>
       <c r="CP10" t="n">
-        <v>0.005680612804685824</v>
+        <v>0.008053006997064105</v>
       </c>
       <c r="CQ10" t="n">
         <v>0</v>
@@ -5910,7 +5910,7 @@
         <v>0</v>
       </c>
       <c r="DL10" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM10" t="n">
         <v>0</v>
@@ -5919,13 +5919,13 @@
         <v>0</v>
       </c>
       <c r="DO10" t="n">
-        <v>26.97487633157158</v>
+        <v>27.74938270756887</v>
       </c>
       <c r="DP10" t="n">
-        <v>0.4600573509409428</v>
+        <v>0.6484937076596962</v>
       </c>
       <c r="DQ10" t="n">
-        <v>0.0700469943332037</v>
+        <v>0.07058387743968812</v>
       </c>
       <c r="DR10" t="n">
         <v>0</v>
@@ -5934,7 +5934,7 @@
         <v>0</v>
       </c>
       <c r="DT10" t="n">
-        <v>17.48181575678515</v>
+        <v>17.99196789382613</v>
       </c>
       <c r="DU10" t="n">
         <v>0</v>
@@ -6014,16 +6014,16 @@
         <v>7</v>
       </c>
       <c r="B11" t="n">
-        <v>12.38702631841619</v>
+        <v>51.0206227831736</v>
       </c>
       <c r="C11" t="n">
-        <v>7.829223284939238</v>
+        <v>36.29627914897833</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>4.557803033476947</v>
+        <v>14.72434363419528</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -6032,16 +6032,16 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>67.52694017561984</v>
+        <v>114.2573010594789</v>
       </c>
       <c r="I11" t="n">
-        <v>19.19652646658173</v>
+        <v>64.42943188051099</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2289191849632906</v>
+        <v>0.3226829235695374</v>
       </c>
       <c r="K11" t="n">
-        <v>48.10149452407482</v>
+        <v>49.50518625539842</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -6281,16 +6281,16 @@
         <v>0</v>
       </c>
       <c r="CM11" t="n">
-        <v>0.02213787888410913</v>
+        <v>0.1026312065067299</v>
       </c>
       <c r="CN11" t="n">
-        <v>0.007034161780892995</v>
+        <v>0.03261037401621993</v>
       </c>
       <c r="CO11" t="n">
         <v>0</v>
       </c>
       <c r="CP11" t="n">
-        <v>0.005452969817673984</v>
+        <v>0.007730293474726031</v>
       </c>
       <c r="CQ11" t="n">
         <v>0</v>
@@ -6356,7 +6356,7 @@
         <v>0</v>
       </c>
       <c r="DL11" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM11" t="n">
         <v>0</v>
@@ -6365,13 +6365,13 @@
         <v>0</v>
       </c>
       <c r="DO11" t="n">
-        <v>28.09338064850041</v>
+        <v>28.9125600674706</v>
       </c>
       <c r="DP11" t="n">
-        <v>0.2289191849632906</v>
+        <v>0.3226829235695374</v>
       </c>
       <c r="DQ11" t="n">
-        <v>0.07764037666585852</v>
+        <v>0.07813865085516734</v>
       </c>
       <c r="DR11" t="n">
         <v>0</v>
@@ -6380,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="DT11" t="n">
-        <v>19.37920407279947</v>
+        <v>19.94472555577557</v>
       </c>
       <c r="DU11" t="n">
         <v>0</v>
@@ -6460,16 +6460,16 @@
         <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>13.65199649143812</v>
+        <v>55.50886057679018</v>
       </c>
       <c r="C12" t="n">
-        <v>9.266384181354702</v>
+        <v>42.95895706476045</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>4.385612310083412</v>
+        <v>12.54990351202973</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -6478,16 +6478,16 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>71.04559050229864</v>
+        <v>118.7417710419446</v>
       </c>
       <c r="I12" t="n">
-        <v>22.66395127102196</v>
+        <v>68.78244388123038</v>
       </c>
       <c r="J12" t="n">
-        <v>0.4358993665413336</v>
+        <v>0.6144407774307891</v>
       </c>
       <c r="K12" t="n">
-        <v>47.94573986473534</v>
+        <v>49.34488638328347</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
@@ -6727,16 +6727,16 @@
         <v>0</v>
       </c>
       <c r="CM12" t="n">
-        <v>0.02620158899990387</v>
+        <v>0.1214705666035543</v>
       </c>
       <c r="CN12" t="n">
-        <v>0.00539090896868146</v>
+        <v>0.02499225397880725</v>
       </c>
       <c r="CO12" t="n">
         <v>0</v>
       </c>
       <c r="CP12" t="n">
-        <v>0.006624467223327889</v>
+        <v>0.009391043314424906</v>
       </c>
       <c r="CQ12" t="n">
         <v>0</v>
@@ -6802,7 +6802,7 @@
         <v>0</v>
       </c>
       <c r="DL12" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM12" t="n">
         <v>0</v>
@@ -6811,13 +6811,13 @@
         <v>0</v>
       </c>
       <c r="DO12" t="n">
-        <v>19.11408142922745</v>
+        <v>19.63207659202659</v>
       </c>
       <c r="DP12" t="n">
-        <v>0.4358993665413336</v>
+        <v>0.6144407774307891</v>
       </c>
       <c r="DQ12" t="n">
-        <v>0.08293501192051581</v>
+        <v>0.08340636528257446</v>
       </c>
       <c r="DR12" t="n">
         <v>0</v>
@@ -6826,7 +6826,7 @@
         <v>0</v>
       </c>
       <c r="DT12" t="n">
-        <v>27.64520019771121</v>
+        <v>28.45193893446481</v>
       </c>
       <c r="DU12" t="n">
         <v>0</v>
@@ -6906,16 +6906,16 @@
         <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>11.25528640141068</v>
+        <v>43.63141255631781</v>
       </c>
       <c r="C13" t="n">
-        <v>7.35163815351133</v>
+        <v>34.08219447967856</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>3.903648247899352</v>
+        <v>9.54921807663926</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -6924,19 +6924,19 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>66.74067914458918</v>
+        <v>113.6179928257156</v>
       </c>
       <c r="I13" t="n">
-        <v>19.73954867922693</v>
+        <v>65.11982459969822</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3297922791184394</v>
+        <v>0.4648729498738348</v>
       </c>
       <c r="K13" t="n">
-        <v>46.67133818624382</v>
+        <v>48.03329527614358</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>-7.105427357601002e-15</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -7173,16 +7173,16 @@
         <v>0</v>
       </c>
       <c r="CM13" t="n">
-        <v>0.0207874611719536</v>
+        <v>0.09637066999317691</v>
       </c>
       <c r="CN13" t="n">
-        <v>0.003418125488835482</v>
+        <v>0.01584642976624129</v>
       </c>
       <c r="CO13" t="n">
         <v>0</v>
       </c>
       <c r="CP13" t="n">
-        <v>0.007276801217738087</v>
+        <v>0.01031581153961969</v>
       </c>
       <c r="CQ13" t="n">
         <v>0</v>
@@ -7248,7 +7248,7 @@
         <v>0</v>
       </c>
       <c r="DL13" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM13" t="n">
         <v>0</v>
@@ -7257,13 +7257,13 @@
         <v>0</v>
       </c>
       <c r="DO13" t="n">
-        <v>17.63021422162677</v>
+        <v>18.14141907977346</v>
       </c>
       <c r="DP13" t="n">
-        <v>0.3297922791184394</v>
+        <v>0.4648729498738348</v>
       </c>
       <c r="DQ13" t="n">
-        <v>0.08982424459972932</v>
+        <v>0.09026056932734516</v>
       </c>
       <c r="DR13" t="n">
         <v>0</v>
@@ -7272,7 +7272,7 @@
         <v>0</v>
       </c>
       <c r="DT13" t="n">
-        <v>27.80740016731077</v>
+        <v>28.61887220306892</v>
       </c>
       <c r="DU13" t="n">
         <v>0</v>
@@ -8309,16 +8309,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>11.25528640141068</v>
+        <v>43.63141255631781</v>
       </c>
       <c r="C4" t="n">
-        <v>7.35163815351133</v>
+        <v>34.08219447967856</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>2.989799390957009</v>
+        <v>7.187665379084021</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -8327,19 +8327,19 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>61.59357552985915</v>
+        <v>107.867153854678</v>
       </c>
       <c r="I4" t="n">
-        <v>17.62779247367044</v>
+        <v>62.47247001385377</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1982666100919121</v>
+        <v>0.2794752628572355</v>
       </c>
       <c r="K4" t="n">
-        <v>40.98856747457172</v>
+        <v>42.18469066808411</v>
       </c>
       <c r="L4" t="n">
-        <v>-7.105427357601002e-15</v>
+        <v>-1.4210854715202e-14</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -8576,16 +8576,16 @@
         <v>0</v>
       </c>
       <c r="CM4" t="n">
-        <v>0.0207874611719536</v>
+        <v>0.09637066999317691</v>
       </c>
       <c r="CN4" t="n">
-        <v>0.002510618403415571</v>
+        <v>0.01163922691823459</v>
       </c>
       <c r="CO4" t="n">
         <v>0</v>
       </c>
       <c r="CP4" t="n">
-        <v>0.005033787163323094</v>
+        <v>0.007136047578270794</v>
       </c>
       <c r="CQ4" t="n">
         <v>0</v>
@@ -8651,7 +8651,7 @@
         <v>0</v>
       </c>
       <c r="DL4" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM4" t="n">
         <v>0</v>
@@ -8660,13 +8660,13 @@
         <v>0</v>
       </c>
       <c r="DO4" t="n">
-        <v>17.63021422162677</v>
+        <v>18.14141907977346</v>
       </c>
       <c r="DP4" t="n">
-        <v>0.1982666100919121</v>
+        <v>0.2794752628572355</v>
       </c>
       <c r="DQ4" t="n">
-        <v>0.04986302666280219</v>
+        <v>0.05050253612232956</v>
       </c>
       <c r="DR4" t="n">
         <v>0</v>
@@ -8675,7 +8675,7 @@
         <v>0</v>
       </c>
       <c r="DT4" t="n">
-        <v>13.49435992054572</v>
+        <v>13.88815062554126</v>
       </c>
       <c r="DU4" t="n">
         <v>0</v>
@@ -8755,16 +8755,16 @@
         <v>0.05</v>
       </c>
       <c r="B5" t="n">
-        <v>11.43778189623505</v>
+        <v>45.36557045742821</v>
       </c>
       <c r="C5" t="n">
-        <v>7.462096469126908</v>
+        <v>34.59427923087236</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>3.163259018089816</v>
+        <v>7.844784384671138</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -8773,19 +8773,19 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>61.88866880505</v>
+        <v>108.4992029591499</v>
       </c>
       <c r="I5" t="n">
-        <v>17.90708437234852</v>
+        <v>62.81284156983486</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2120602687840324</v>
+        <v>0.2989187101777714</v>
       </c>
       <c r="K5" t="n">
-        <v>41.94100165705288</v>
+        <v>43.16491866445414</v>
       </c>
       <c r="L5" t="n">
-        <v>-7.105427357601002e-15</v>
+        <v>-1.4210854715202e-14</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -9022,16 +9022,16 @@
         <v>0</v>
       </c>
       <c r="CM5" t="n">
-        <v>0.02109979264135291</v>
+        <v>0.0978186386853121</v>
       </c>
       <c r="CN5" t="n">
-        <v>0.002834105001354396</v>
+        <v>0.01313891078627898</v>
       </c>
       <c r="CO5" t="n">
         <v>0</v>
       </c>
       <c r="CP5" t="n">
-        <v>0.005096094906958807</v>
+        <v>0.007224376903419621</v>
       </c>
       <c r="CQ5" t="n">
         <v>0</v>
@@ -9097,7 +9097,7 @@
         <v>0</v>
       </c>
       <c r="DL5" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM5" t="n">
         <v>0</v>
@@ -9106,13 +9106,13 @@
         <v>0</v>
       </c>
       <c r="DO5" t="n">
-        <v>18.29795446504708</v>
+        <v>18.81221496028737</v>
       </c>
       <c r="DP5" t="n">
-        <v>0.2120602687840324</v>
+        <v>0.2989187101777714</v>
       </c>
       <c r="DQ5" t="n">
-        <v>0.05383944715836328</v>
+        <v>0.05445873831689609</v>
       </c>
       <c r="DR5" t="n">
         <v>0</v>
@@ -9121,7 +9121,7 @@
         <v>0</v>
       </c>
       <c r="DT5" t="n">
-        <v>15.20854096194042</v>
+        <v>15.65235468134756</v>
       </c>
       <c r="DU5" t="n">
         <v>0</v>
@@ -9201,16 +9201,16 @@
         <v>0.25</v>
       </c>
       <c r="B6" t="n">
-        <v>11.87429854891985</v>
+        <v>48.23602865765493</v>
       </c>
       <c r="C6" t="n">
-        <v>7.883576733128921</v>
+        <v>36.5482617347857</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>3.544060846645691</v>
+        <v>9.554879245896823</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -9219,19 +9219,19 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>63.90722550724593</v>
+        <v>110.438070092443</v>
       </c>
       <c r="I6" t="n">
-        <v>19.33228201974303</v>
+        <v>64.6020300603078</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2885021073384794</v>
+        <v>0.4066706050298127</v>
       </c>
       <c r="K6" t="n">
-        <v>43.77977119164484</v>
+        <v>45.05734693911341</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>-7.105427357601002e-15</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -9468,16 +9468,16 @@
         <v>0</v>
       </c>
       <c r="CM6" t="n">
-        <v>0.0222915684659699</v>
+        <v>0.1033437114082364</v>
       </c>
       <c r="CN6" t="n">
-        <v>0.003582357412000444</v>
+        <v>0.01660780896203406</v>
       </c>
       <c r="CO6" t="n">
         <v>0</v>
       </c>
       <c r="CP6" t="n">
-        <v>0.005476475753900424</v>
+        <v>0.007763616194547371</v>
       </c>
       <c r="CQ6" t="n">
         <v>0</v>
@@ -9543,7 +9543,7 @@
         <v>0</v>
       </c>
       <c r="DL6" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM6" t="n">
         <v>0</v>
@@ -9552,13 +9552,13 @@
         <v>0</v>
       </c>
       <c r="DO6" t="n">
-        <v>20.79973078892063</v>
+        <v>21.36489495852309</v>
       </c>
       <c r="DP6" t="n">
-        <v>0.2885021073384794</v>
+        <v>0.4066706050298127</v>
       </c>
       <c r="DQ6" t="n">
-        <v>0.06640964731638184</v>
+        <v>0.06696502468847269</v>
       </c>
       <c r="DR6" t="n">
         <v>0</v>
@@ -9567,7 +9567,7 @@
         <v>0</v>
       </c>
       <c r="DT6" t="n">
-        <v>17.73296987256749</v>
+        <v>18.2504511572597</v>
       </c>
       <c r="DU6" t="n">
         <v>0</v>
@@ -9647,16 +9647,16 @@
         <v>0.5</v>
       </c>
       <c r="B7" t="n">
-        <v>12.27366420889142</v>
+        <v>50.20465928941221</v>
       </c>
       <c r="C7" t="n">
-        <v>8.33143380526915</v>
+        <v>38.62452712122777</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>4.280805635664132</v>
+        <v>12.51220861120615</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -9665,16 +9665,16 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>67.39801418014559</v>
+        <v>114.4317549272162</v>
       </c>
       <c r="I7" t="n">
-        <v>21.18283136854265</v>
+        <v>66.92622966883752</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3404600945283929</v>
+        <v>0.4799102297992195</v>
       </c>
       <c r="K7" t="n">
-        <v>45.98479889238526</v>
+        <v>47.32672147941659</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -9914,16 +9914,16 @@
         <v>0</v>
       </c>
       <c r="CM7" t="n">
-        <v>0.02355792724251728</v>
+        <v>0.1092145506963101</v>
       </c>
       <c r="CN7" t="n">
-        <v>0.005485300477228217</v>
+        <v>0.02542985301243001</v>
       </c>
       <c r="CO7" t="n">
         <v>0</v>
       </c>
       <c r="CP7" t="n">
-        <v>0.005771006931708646</v>
+        <v>0.00818115242123521</v>
       </c>
       <c r="CQ7" t="n">
         <v>0</v>
@@ -9989,7 +9989,7 @@
         <v>0</v>
       </c>
       <c r="DL7" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM7" t="n">
         <v>0</v>
@@ -9998,13 +9998,13 @@
         <v>0</v>
       </c>
       <c r="DO7" t="n">
-        <v>25.85331266287736</v>
+        <v>26.59003182001995</v>
       </c>
       <c r="DP7" t="n">
-        <v>0.3404600945283929</v>
+        <v>0.4799102297992195</v>
       </c>
       <c r="DQ7" t="n">
-        <v>0.07469037541289528</v>
+        <v>0.07520364902526144</v>
       </c>
       <c r="DR7" t="n">
         <v>0</v>
@@ -10013,7 +10013,7 @@
         <v>0</v>
       </c>
       <c r="DT7" t="n">
-        <v>18.85240583198907</v>
+        <v>19.40255435530937</v>
       </c>
       <c r="DU7" t="n">
         <v>0</v>
@@ -10093,16 +10093,16 @@
         <v>0.75</v>
       </c>
       <c r="B8" t="n">
-        <v>12.85229046728324</v>
+        <v>52.94085168974452</v>
       </c>
       <c r="C8" t="n">
-        <v>8.851169245271478</v>
+        <v>41.03402062107857</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>4.533484027771574</v>
+        <v>14.06536733871983</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -10111,16 +10111,16 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>70.24503483570835</v>
+        <v>118.0107789287259</v>
       </c>
       <c r="I8" t="n">
-        <v>22.91003514714467</v>
+        <v>69.10685089920931</v>
       </c>
       <c r="J8" t="n">
-        <v>0.4002905362713555</v>
+        <v>0.5642468128740369</v>
       </c>
       <c r="K8" t="n">
-        <v>48.06255585923995</v>
+        <v>49.46511128736968</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -10360,16 +10360,16 @@
         <v>0</v>
       </c>
       <c r="CM8" t="n">
-        <v>0.02502752899020075</v>
+        <v>0.1160276243985707</v>
       </c>
       <c r="CN8" t="n">
-        <v>0.006559605785216168</v>
+        <v>0.03041033242026215</v>
       </c>
       <c r="CO8" t="n">
         <v>0</v>
       </c>
       <c r="CP8" t="n">
-        <v>0.006251258944386314</v>
+        <v>0.008861972070702814</v>
       </c>
       <c r="CQ8" t="n">
         <v>0</v>
@@ -10435,7 +10435,7 @@
         <v>0</v>
       </c>
       <c r="DL8" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM8" t="n">
         <v>0</v>
@@ -10444,13 +10444,13 @@
         <v>0</v>
       </c>
       <c r="DO8" t="n">
-        <v>29.14361431373031</v>
+        <v>29.96340353559551</v>
       </c>
       <c r="DP8" t="n">
-        <v>0.4002905362713555</v>
+        <v>0.5642468128740369</v>
       </c>
       <c r="DQ8" t="n">
-        <v>0.08810193642992595</v>
+        <v>0.08854701831615248</v>
       </c>
       <c r="DR8" t="n">
         <v>0</v>
@@ -10459,7 +10459,7 @@
         <v>0</v>
       </c>
       <c r="DT8" t="n">
-        <v>19.78881713479137</v>
+        <v>20.36629189435168</v>
       </c>
       <c r="DU8" t="n">
         <v>0</v>
@@ -10539,16 +10539,16 @@
         <v>0.95</v>
       </c>
       <c r="B9" t="n">
-        <v>13.51289112271557</v>
+        <v>55.43353927927879</v>
       </c>
       <c r="C9" t="n">
-        <v>9.192814942423054</v>
+        <v>42.6178900730733</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>4.562487274911933</v>
+        <v>15.00489196638351</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -10557,19 +10557,19 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>73.5074235139822</v>
+        <v>121.3757975201252</v>
       </c>
       <c r="I9" t="n">
-        <v>24.11480316844394</v>
+        <v>70.62828985005029</v>
       </c>
       <c r="J9" t="n">
-        <v>0.4491862579611187</v>
+        <v>0.6331698890566879</v>
       </c>
       <c r="K9" t="n">
-        <v>49.94036912207167</v>
+        <v>51.39772265940958</v>
       </c>
       <c r="L9" t="n">
-        <v>3.907985046680543e-15</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -10806,16 +10806,16 @@
         <v>0</v>
       </c>
       <c r="CM9" t="n">
-        <v>0.02599356492883183</v>
+        <v>0.1205061670100644</v>
       </c>
       <c r="CN9" t="n">
-        <v>0.007270456174915729</v>
+        <v>0.03370583482690932</v>
       </c>
       <c r="CO9" t="n">
         <v>0</v>
       </c>
       <c r="CP9" t="n">
-        <v>0.006983250920253497</v>
+        <v>0.009899665838282038</v>
       </c>
       <c r="CQ9" t="n">
         <v>0</v>
@@ -10881,7 +10881,7 @@
         <v>0</v>
       </c>
       <c r="DL9" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM9" t="n">
         <v>0</v>
@@ -10890,13 +10890,13 @@
         <v>0</v>
       </c>
       <c r="DO9" t="n">
-        <v>31.67908848945565</v>
+        <v>32.58958482284296</v>
       </c>
       <c r="DP9" t="n">
-        <v>0.4491862579611187</v>
+        <v>0.6331698890566879</v>
       </c>
       <c r="DQ9" t="n">
-        <v>0.1007478849743259</v>
+        <v>0.1011286679278017</v>
       </c>
       <c r="DR9" t="n">
         <v>0</v>
@@ -10905,7 +10905,7 @@
         <v>0</v>
       </c>
       <c r="DT9" t="n">
-        <v>27.73441018099097</v>
+        <v>28.54375223219708</v>
       </c>
       <c r="DU9" t="n">
         <v>0</v>
@@ -10985,16 +10985,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>13.65199649143812</v>
+        <v>55.50886057679018</v>
       </c>
       <c r="C10" t="n">
-        <v>9.266384181354702</v>
+        <v>42.95895706476045</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>4.56320102226515</v>
+        <v>15.23443151090117</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -11003,19 +11003,19 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>74.02453503439295</v>
+        <v>121.8121045053803</v>
       </c>
       <c r="I10" t="n">
-        <v>24.46354123910693</v>
+        <v>71.06755766119238</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4600573509409428</v>
+        <v>0.6484937076596962</v>
       </c>
       <c r="K10" t="n">
-        <v>50.8342053184488</v>
+        <v>52.31764267065415</v>
       </c>
       <c r="L10" t="n">
-        <v>7.105427357601002e-15</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -11252,16 +11252,16 @@
         <v>0</v>
       </c>
       <c r="CM10" t="n">
-        <v>0.02620158899990387</v>
+        <v>0.1214705666035543</v>
       </c>
       <c r="CN10" t="n">
-        <v>0.007463787951843422</v>
+        <v>0.0346021209447461</v>
       </c>
       <c r="CO10" t="n">
         <v>0</v>
       </c>
       <c r="CP10" t="n">
-        <v>0.007276801217738087</v>
+        <v>0.01031581153961969</v>
       </c>
       <c r="CQ10" t="n">
         <v>0</v>
@@ -11327,7 +11327,7 @@
         <v>0</v>
       </c>
       <c r="DL10" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="DM10" t="n">
         <v>0</v>
@@ -11336,13 +11336,13 @@
         <v>0</v>
       </c>
       <c r="DO10" t="n">
-        <v>31.97965694956584</v>
+        <v>32.90304280249227</v>
       </c>
       <c r="DP10" t="n">
-        <v>0.4600573509409428</v>
+        <v>0.6484937076596962</v>
       </c>
       <c r="DQ10" t="n">
-        <v>0.1035936374226998</v>
+        <v>0.1039599510111723</v>
       </c>
       <c r="DR10" t="n">
         <v>0</v>
@@ -11351,7 +11351,7 @@
         <v>0</v>
       </c>
       <c r="DT10" t="n">
-        <v>27.80740016731077</v>
+        <v>28.61887220306892</v>
       </c>
       <c r="DU10" t="n">
         <v>0</v>
@@ -11544,19 +11544,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.2242424242424242</v>
+        <v>0.2</v>
       </c>
       <c r="D2" t="n">
         <v>-0.04242424242424241</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>0.2</v>
+        <v>0.3212121212121212</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
-        <v>0.4787878787878787</v>
+        <v>0.4424242424242424</v>
       </c>
       <c r="J2" t="n">
         <v>0.2363636363636363</v>
@@ -11568,7 +11568,7 @@
         <v>0.4666666666666666</v>
       </c>
       <c r="M2" t="n">
-        <v>0.3370999312316211</v>
+        <v>-0.4403855060505442</v>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
@@ -11581,19 +11581,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.06666666666666665</v>
+        <v>0.05454545454545454</v>
       </c>
       <c r="D3" t="n">
         <v>-0.2363636363636363</v>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>0.2363636363636363</v>
+        <v>0.406060606060606</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>0.309090909090909</v>
+        <v>0.2606060606060606</v>
       </c>
       <c r="J3" t="n">
         <v>0.2363636363636363</v>
@@ -11605,7 +11605,7 @@
         <v>0.2121212121212121</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2097510683218975</v>
+        <v>-0.5504818825631803</v>
       </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
@@ -11618,19 +11618,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.2121212121212121</v>
+        <v>0.2848484848484849</v>
       </c>
       <c r="D4" t="n">
         <v>0.1515151515151515</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.103030303030303</v>
+        <v>0.2121212121212121</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>0.4303030303030302</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="J4" t="n">
         <v>0.2727272727272727</v>
@@ -11642,7 +11642,7 @@
         <v>0.3212121212121212</v>
       </c>
       <c r="M4" t="n">
-        <v>0.7491109582924913</v>
+        <v>-0.3302891295379082</v>
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
@@ -11655,19 +11655,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.4666666666666666</v>
+        <v>-0.4303030303030302</v>
       </c>
       <c r="D5" t="n">
         <v>-0.4787878787878787</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>-0.103030303030303</v>
+        <v>-0.1878787878787879</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
-        <v>0.05454545454545454</v>
+        <v>0.07878787878787878</v>
       </c>
       <c r="J5" t="n">
         <v>-0.1272727272727273</v>
@@ -11679,7 +11679,7 @@
         <v>0.4545454545454545</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2172421779048224</v>
+        <v>-0.05504818825631803</v>
       </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
@@ -11692,19 +11692,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.5878787878787878</v>
+        <v>-0.6606060606060605</v>
       </c>
       <c r="D6" t="n">
         <v>-0.4666666666666666</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>-0.2969696969696969</v>
+        <v>-0.5030303030303029</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>-0.5393939393939393</v>
+        <v>-0.5757575757575757</v>
       </c>
       <c r="J6" t="n">
         <v>-0.5757575757575757</v>
@@ -11716,7 +11716,7 @@
         <v>-0.07878787878787878</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.6741998624632421</v>
+        <v>0.3853373177942261</v>
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
@@ -11729,19 +11729,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.09090909090909088</v>
+        <v>0.1515151515151515</v>
       </c>
       <c r="D7" t="n">
         <v>-0.1878787878787879</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>0.06666666666666665</v>
+        <v>0.2606060606060606</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>0.3696969696969697</v>
+        <v>0.3212121212121212</v>
       </c>
       <c r="J7" t="n">
         <v>0.3575757575757575</v>
@@ -11753,7 +11753,7 @@
         <v>0.2606060606060606</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.09738442457802386</v>
+        <v>-0.1926686588971131</v>
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -11766,19 +11766,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.05454545454545454</v>
+        <v>-0.006060606060606061</v>
       </c>
       <c r="D8" t="n">
         <v>0.3939393939393939</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>-0.1151515151515151</v>
+        <v>-0.2484848484848484</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>-0.4424242424242424</v>
+        <v>-0.4181818181818182</v>
       </c>
       <c r="J8" t="n">
         <v>-0.3575757575757575</v>
@@ -11790,7 +11790,7 @@
         <v>-0.4545454545454545</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.1498221916584982</v>
+        <v>0.3578132236660672</v>
       </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
@@ -11803,19 +11803,19 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.4424242424242424</v>
+        <v>-0.4303030303030302</v>
       </c>
       <c r="D9" t="n">
         <v>0.0303030303030303</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>-0.3939393939393939</v>
+        <v>-0.309090909090909</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>-0.4666666666666666</v>
+        <v>-0.4181818181818182</v>
       </c>
       <c r="J9" t="n">
         <v>-0.2727272727272727</v>
@@ -11827,7 +11827,7 @@
         <v>-0.5393939393939393</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.03745554791462456</v>
+        <v>-0.2201927530252721</v>
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
@@ -11840,19 +11840,19 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.4303030303030302</v>
+        <v>-0.3818181818181818</v>
       </c>
       <c r="D10" t="n">
         <v>0.4181818181818182</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>-0.8545454545454544</v>
+        <v>-0.8424242424242423</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
-        <v>-0.5636363636363636</v>
+        <v>-0.4909090909090909</v>
       </c>
       <c r="J10" t="n">
         <v>-0.4666666666666666</v>
@@ -11864,7 +11864,7 @@
         <v>-0.4424242424242424</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.4719399037242695</v>
+        <v>0.5229577884350213</v>
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -11877,19 +11877,19 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.103030303030303</v>
+        <v>0.2</v>
       </c>
       <c r="D11" t="n">
         <v>0.0303030303030303</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>0.09090909090909088</v>
+        <v>0.4424242424242424</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
-        <v>0.3212121212121212</v>
+        <v>0.2969696969696969</v>
       </c>
       <c r="J11" t="n">
         <v>0.09090909090909088</v>
@@ -11901,7 +11901,7 @@
         <v>0.2606060606060606</v>
       </c>
       <c r="M11" t="n">
-        <v>0.4045199174779453</v>
+        <v>-0.1100963765126361</v>
       </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
@@ -11914,19 +11914,19 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.1515151515151515</v>
+        <v>-0.1757575757575758</v>
       </c>
       <c r="D12" t="n">
         <v>0.2121212121212121</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>-0.2727272727272727</v>
+        <v>-0.5636363636363636</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>-0.4424242424242424</v>
+        <v>-0.3696969696969697</v>
       </c>
       <c r="J12" t="n">
         <v>-0.1878787878787879</v>
@@ -11938,7 +11938,7 @@
         <v>-0.4303030303030302</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.2022599587389727</v>
+        <v>0.3027650354097491</v>
       </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
@@ -11951,19 +11951,19 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.006060606060606061</v>
+        <v>-0.05454545454545454</v>
       </c>
       <c r="D13" t="n">
         <v>-0.6727272727272726</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>0.5393939393939393</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
-        <v>0.3696969696969697</v>
+        <v>0.2848484848484849</v>
       </c>
       <c r="J13" t="n">
         <v>0.0303030303030303</v>
@@ -11975,7 +11975,7 @@
         <v>0.6484848484848483</v>
       </c>
       <c r="M13" t="n">
-        <v>0.3370999312316211</v>
+        <v>-0.3027650354097491</v>
       </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -11988,19 +11988,19 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.709090909090909</v>
+        <v>-0.7696969696969697</v>
       </c>
       <c r="D14" t="n">
         <v>-0.6484848484848483</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>-0.1515151515151515</v>
+        <v>-0.2</v>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>-0.4787878787878787</v>
+        <v>-0.5272727272727272</v>
       </c>
       <c r="J14" t="n">
         <v>-0.7575757575757575</v>
@@ -12012,7 +12012,7 @@
         <v>0.06666666666666665</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.1123666437438737</v>
+        <v>0.08257228238447704</v>
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
@@ -12025,19 +12025,19 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.06666666666666665</v>
+        <v>-0.006060606060606061</v>
       </c>
       <c r="D15" t="n">
         <v>0.1151515151515151</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>0.2</v>
+        <v>0.103030303030303</v>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
-        <v>-0.3696969696969697</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="J15" t="n">
         <v>0.0303030303030303</v>
@@ -12049,7 +12049,7 @@
         <v>-0.7333333333333332</v>
       </c>
       <c r="M15" t="n">
-        <v>0.02996443833169965</v>
+        <v>-0.3302891295379082</v>
       </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
@@ -12062,19 +12062,19 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.1878787878787879</v>
+        <v>-0.2242424242424242</v>
       </c>
       <c r="D16" t="n">
         <v>-0.406060606060606</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>0.3454545454545455</v>
+        <v>0.3212121212121212</v>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
-        <v>-0.3212121212121212</v>
+        <v>-0.3696969696969697</v>
       </c>
       <c r="J16" t="n">
         <v>-0.406060606060606</v>
@@ -12086,7 +12086,7 @@
         <v>-0.1636363636363636</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1573133012414231</v>
+        <v>0.08257228238447704</v>
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
@@ -12099,19 +12099,19 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.4666666666666666</v>
       </c>
       <c r="D17" t="n">
         <v>0.3818181818181818</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>0.06666666666666665</v>
+        <v>0.1757575757575758</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
-        <v>0.6606060606060605</v>
+        <v>0.6969696969696969</v>
       </c>
       <c r="J17" t="n">
         <v>0.6</v>
@@ -12123,7 +12123,7 @@
         <v>0.5151515151515151</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>-0.1651445647689541</v>
       </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
@@ -12136,19 +12136,19 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.3212121212121212</v>
+        <v>0.2</v>
       </c>
       <c r="D18" t="n">
         <v>0.4181818181818182</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>0.06666666666666665</v>
+        <v>-0.103030303030303</v>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
-        <v>-0.2121212121212121</v>
+        <v>-0.1878787878787879</v>
       </c>
       <c r="J18" t="n">
         <v>0.06666666666666665</v>
@@ -12160,7 +12160,7 @@
         <v>-0.4666666666666666</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.42699324622672</v>
+        <v>0.05504818825631803</v>
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
@@ -12177,19 +12177,19 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.05454545454545454</v>
+        <v>0.1636363636363636</v>
       </c>
       <c r="D19" t="n">
         <v>-0.1878787878787879</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>0.06666666666666665</v>
+        <v>0.2969696969696969</v>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.4666666666666666</v>
       </c>
       <c r="J19" t="n">
         <v>0.07878787878787878</v>
@@ -12201,7 +12201,7 @@
         <v>0.7818181818181817</v>
       </c>
       <c r="M19" t="n">
-        <v>0.2172421779048224</v>
+        <v>0.2477168471534311</v>
       </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
@@ -12226,7 +12226,7 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
-        <v>-0.04242424242424241</v>
+        <v>-0.1151515151515151</v>
       </c>
       <c r="J20" t="n">
         <v>-0.4303030303030302</v>
@@ -12238,7 +12238,7 @@
         <v>0.3454545454545455</v>
       </c>
       <c r="M20" t="n">
-        <v>0.2996443833169965</v>
+        <v>0.1100963765126361</v>
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
@@ -12251,19 +12251,19 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.0303030303030303</v>
+        <v>0.04242424242424241</v>
       </c>
       <c r="D21" t="n">
         <v>-0.0303030303030303</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>-0.1151515151515151</v>
+        <v>0.07878787878787878</v>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
-        <v>0.2848484848484849</v>
+        <v>0.2484848484848484</v>
       </c>
       <c r="J21" t="n">
         <v>-0.2121212121212121</v>
@@ -12275,7 +12275,7 @@
         <v>0.6</v>
       </c>
       <c r="M21" t="n">
-        <v>0.2846621641511467</v>
+        <v>0.2752409412815902</v>
       </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
@@ -12288,19 +12288,19 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.1272727272727273</v>
+        <v>-0.2484848484848484</v>
       </c>
       <c r="D22" t="n">
         <v>-0.2727272727272727</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>0.2242424242424242</v>
+        <v>0.1515151515151515</v>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
-        <v>-0.1878787878787879</v>
+        <v>-0.2</v>
       </c>
       <c r="J22" t="n">
         <v>-0.06666666666666665</v>
@@ -12312,7 +12312,7 @@
         <v>-0.2727272727272727</v>
       </c>
       <c r="M22" t="n">
-        <v>0.07491109582924912</v>
+        <v>-0.6055300708194983</v>
       </c>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
@@ -12325,19 +12325,19 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.006060606060606061</v>
+        <v>0.0303030303030303</v>
       </c>
       <c r="D23" t="n">
         <v>0.5272727272727272</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>-0.4424242424242424</v>
+        <v>-0.2848484848484849</v>
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
-        <v>-0.3454545454545455</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="J23" t="n">
         <v>-0.2484848484848484</v>
@@ -12349,7 +12349,7 @@
         <v>-0.4787878787878787</v>
       </c>
       <c r="M23" t="n">
-        <v>-0.4120110270608701</v>
+        <v>0.3853373177942261</v>
       </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
@@ -12362,19 +12362,19 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.0303030303030303</v>
+        <v>0.1636363636363636</v>
       </c>
       <c r="D24" t="n">
         <v>0.103030303030303</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>-0.2242424242424242</v>
+        <v>0.05454545454545454</v>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>0.1757575757575758</v>
+        <v>0.1515151515151515</v>
       </c>
       <c r="J24" t="n">
         <v>0.1272727272727273</v>
@@ -12386,7 +12386,7 @@
         <v>0.006060606060606061</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1872777395731228</v>
+        <v>-0.02752409412815901</v>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
@@ -12403,19 +12403,19 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.06666666666666665</v>
+        <v>-0.01818181818181818</v>
       </c>
       <c r="D25" t="n">
         <v>0.309090909090909</v>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>-0.103030303030303</v>
+        <v>-0.2969696969696969</v>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>-0.3575757575757575</v>
+        <v>-0.3212121212121212</v>
       </c>
       <c r="J25" t="n">
         <v>-0.0303030303030303</v>
@@ -12427,7 +12427,7 @@
         <v>-0.5030303030303029</v>
       </c>
       <c r="M25" t="n">
-        <v>-0.4794310133071943</v>
+        <v>0.1376204706407951</v>
       </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
@@ -12440,19 +12440,19 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.3212121212121212</v>
+        <v>0.1878787878787879</v>
       </c>
       <c r="D26" t="n">
         <v>0.2606060606060606</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>0.2</v>
+        <v>-0.06666666666666665</v>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
-        <v>-0.1757575757575758</v>
+        <v>-0.1393939393939394</v>
       </c>
       <c r="J26" t="n">
         <v>0.3454545454545455</v>
@@ -12464,7 +12464,7 @@
         <v>-0.6121212121212121</v>
       </c>
       <c r="M26" t="n">
-        <v>-0.3520821503974709</v>
+        <v>-0.3302891295379082</v>
       </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
@@ -12484,12 +12484,12 @@
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>-0.4545454545454545</v>
+        <v>-0.4424242424242424</v>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
-        <v>-0.5757575757575757</v>
+        <v>-0.6</v>
       </c>
       <c r="J27" t="n">
         <v>-0.8666666666666665</v>
@@ -12501,7 +12501,7 @@
         <v>-0.1151515151515151</v>
       </c>
       <c r="M27" t="n">
-        <v>-0.2172421779048224</v>
+        <v>0.6330541649476573</v>
       </c>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
@@ -12514,19 +12514,19 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.2727272727272727</v>
+        <v>-0.2848484848484849</v>
       </c>
       <c r="D28" t="n">
         <v>-0.5636363636363636</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>0.2</v>
+        <v>0.3212121212121212</v>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>-0.1272727272727273</v>
+        <v>-0.2121212121212121</v>
       </c>
       <c r="J28" t="n">
         <v>-0.2</v>
@@ -12538,7 +12538,7 @@
         <v>-0.1151515151515151</v>
       </c>
       <c r="M28" t="n">
-        <v>0.2996443833169965</v>
+        <v>-0.4954336943068622</v>
       </c>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
@@ -12551,19 +12551,19 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.5393939393939393</v>
+        <v>-0.6242424242424242</v>
       </c>
       <c r="D29" t="n">
         <v>-0.6121212121212121</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
-        <v>0.1393939393939394</v>
+        <v>-0.07878787878787878</v>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>-0.6484848484848483</v>
+        <v>-0.6727272727272726</v>
       </c>
       <c r="J29" t="n">
         <v>-0.5878787878787878</v>
@@ -12575,7 +12575,7 @@
         <v>-0.4424242424242424</v>
       </c>
       <c r="M29" t="n">
-        <v>0.172295520407273</v>
+        <v>-0.1926686588971131</v>
       </c>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
@@ -12588,19 +12588,19 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.1515151515151515</v>
+        <v>-0.103030303030303</v>
       </c>
       <c r="D30" t="n">
         <v>0.1151515151515151</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>-0.3818181818181818</v>
+        <v>-0.3333333333333333</v>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="n">
-        <v>-0.1393939393939394</v>
+        <v>-0.1757575757575758</v>
       </c>
       <c r="J30" t="n">
         <v>-0.4303030303030302</v>
@@ -12612,7 +12612,7 @@
         <v>0.1878787878787879</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.2022599587389727</v>
+        <v>0.6330541649476573</v>
       </c>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
@@ -12625,19 +12625,19 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.4909090909090909</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="D31" t="n">
         <v>0.2121212121212121</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>0.4787878787878787</v>
+        <v>0.5636363636363636</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>0.3696969696969697</v>
+        <v>0.3818181818181818</v>
       </c>
       <c r="J31" t="n">
         <v>0.3575757575757575</v>
@@ -12649,7 +12649,7 @@
         <v>0.05454545454545454</v>
       </c>
       <c r="M31" t="n">
-        <v>0.6741998624632421</v>
+        <v>-0.3027650354097491</v>
       </c>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr"/>
@@ -12662,19 +12662,19 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.8060606060606059</v>
+        <v>0.8303030303030302</v>
       </c>
       <c r="D32" t="n">
         <v>0.5030303030303029</v>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>0.3212121212121212</v>
+        <v>0.3696969696969697</v>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
-        <v>0.7696969696969697</v>
+        <v>0.8060606060606059</v>
       </c>
       <c r="J32" t="n">
         <v>0.9878787878787878</v>
@@ -12686,7 +12686,7 @@
         <v>0.2242424242424242</v>
       </c>
       <c r="M32" t="n">
-        <v>0.1573133012414231</v>
+        <v>-0.3853373177942261</v>
       </c>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
@@ -12699,19 +12699,19 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.0303030303030303</v>
+        <v>0.09090909090909088</v>
       </c>
       <c r="D33" t="n">
         <v>0.309090909090909</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>-0.2363636363636363</v>
+        <v>-0.406060606060606</v>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
-        <v>-0.0303030303030303</v>
+        <v>0.07878787878787878</v>
       </c>
       <c r="J33" t="n">
         <v>0.2969696969696969</v>
@@ -12723,7 +12723,7 @@
         <v>-0.2</v>
       </c>
       <c r="M33" t="n">
-        <v>-0.08240220541217404</v>
+        <v>0.1651445647689541</v>
       </c>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
@@ -12736,19 +12736,19 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.1515151515151515</v>
+        <v>-0.1151515151515151</v>
       </c>
       <c r="D34" t="n">
         <v>-0.0303030303030303</v>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>-0.1878787878787879</v>
+        <v>-0.3696969696969697</v>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>-0.09090909090909088</v>
+        <v>-0.05454545454545454</v>
       </c>
       <c r="J34" t="n">
         <v>-0.05454545454545454</v>
@@ -12760,7 +12760,7 @@
         <v>0.1272727272727273</v>
       </c>
       <c r="M34" t="n">
-        <v>-0.2771710545682217</v>
+        <v>0.4954336943068622</v>
       </c>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
@@ -12773,19 +12773,19 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.5757575757575757</v>
+        <v>-0.5272727272727272</v>
       </c>
       <c r="D35" t="n">
         <v>-0.01818181818181818</v>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="n">
-        <v>-0.5515151515151515</v>
+        <v>-0.4424242424242424</v>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="n">
-        <v>-0.2969696969696969</v>
+        <v>-0.2363636363636363</v>
       </c>
       <c r="J35" t="n">
         <v>-0.3696969696969697</v>
@@ -12797,7 +12797,7 @@
         <v>-0.06666666666666665</v>
       </c>
       <c r="M35" t="n">
-        <v>0.01498221916584982</v>
+        <v>0</v>
       </c>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
@@ -12810,19 +12810,19 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>-0.4424242424242424</v>
+        <v>-0.4666666666666666</v>
       </c>
       <c r="D36" t="n">
         <v>-0.5515151515151515</v>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
-        <v>0.06666666666666665</v>
+        <v>0.1515151515151515</v>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="n">
-        <v>-0.09090909090909088</v>
+        <v>-0.1272727272727273</v>
       </c>
       <c r="J36" t="n">
         <v>-0.2848484848484849</v>
@@ -12834,7 +12834,7 @@
         <v>0.1393939393939394</v>
       </c>
       <c r="M36" t="n">
-        <v>0.3370999312316211</v>
+        <v>-0.4679096001787033</v>
       </c>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
@@ -12847,19 +12847,19 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-0.5878787878787878</v>
+        <v>-0.6121212121212121</v>
       </c>
       <c r="D37" t="n">
         <v>-0.4787878787878787</v>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>0.04242424242424241</v>
+        <v>-0.07878787878787878</v>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="n">
-        <v>-0.5757575757575757</v>
+        <v>-0.5515151515151515</v>
       </c>
       <c r="J37" t="n">
         <v>-0.5515151515151515</v>
@@ -12871,7 +12871,7 @@
         <v>-0.3575757575757575</v>
       </c>
       <c r="M37" t="n">
-        <v>0.3520821503974709</v>
+        <v>-0.1376204706407951</v>
       </c>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
@@ -12888,19 +12888,19 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.5636363636363636</v>
+        <v>0.6363636363636362</v>
       </c>
       <c r="D38" t="n">
         <v>0.9999999999999999</v>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>-0.3696969696969697</v>
+        <v>-0.2242424242424242</v>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="n">
-        <v>0.3454545454545455</v>
+        <v>0.4181818181818182</v>
       </c>
       <c r="J38" t="n">
         <v>0.4303030303030302</v>
@@ -12912,7 +12912,7 @@
         <v>0.01818181818181818</v>
       </c>
       <c r="M38" t="n">
-        <v>-0.2247332874877473</v>
+        <v>0.3578132236660672</v>
       </c>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
@@ -12925,19 +12925,19 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.5272727272727272</v>
+        <v>0.4666666666666666</v>
       </c>
       <c r="D39" t="n">
         <v>-0.3333333333333333</v>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>0.9151515151515152</v>
+        <v>0.9757575757575757</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
-        <v>0.5030303030303029</v>
+        <v>0.406060606060606</v>
       </c>
       <c r="J39" t="n">
         <v>0.3818181818181818</v>
@@ -12949,7 +12949,7 @@
         <v>0.309090909090909</v>
       </c>
       <c r="M39" t="n">
-        <v>0.4719399037242695</v>
+        <v>-0.4954336943068622</v>
       </c>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
@@ -14270,16 +14270,16 @@
         <v>0.05204398232549917</v>
       </c>
       <c r="AN4" t="n">
-        <v>12.93363662479974</v>
+        <v>53.07492191862304</v>
       </c>
       <c r="AO4" t="n">
-        <v>8.75763766355489</v>
+        <v>40.60040820824047</v>
       </c>
       <c r="AP4" t="n">
         <v>0</v>
       </c>
       <c r="AQ4" t="n">
-        <v>4.175998961244851</v>
+        <v>12.47451371038257</v>
       </c>
       <c r="AR4" t="n">
         <v>0</v>
@@ -14288,19 +14288,19 @@
         <v>0</v>
       </c>
       <c r="AT4" t="n">
-        <v>72.87539832236907</v>
+        <v>120.8425334270357</v>
       </c>
       <c r="AU4" t="n">
-        <v>23.68856774874473</v>
+        <v>70.09140696976552</v>
       </c>
       <c r="AV4" t="n">
-        <v>0.338927913791387</v>
+        <v>0.4777504782706036</v>
       </c>
       <c r="AW4" t="n">
-        <v>48.84790265983295</v>
+        <v>50.27337597899956</v>
       </c>
       <c r="AX4" t="n">
-        <v>-7.105427357601002e-15</v>
+        <v>0</v>
       </c>
       <c r="AY4" t="n">
         <v>0</v>
@@ -14537,16 +14537,16 @@
         <v>0</v>
       </c>
       <c r="DY4" t="n">
-        <v>0.02476305948249567</v>
+        <v>0.1148015437608499</v>
       </c>
       <c r="DZ4" t="n">
-        <v>0.005579691985774974</v>
+        <v>0.02586745204605278</v>
       </c>
       <c r="EA4" t="n">
         <v>0</v>
       </c>
       <c r="EB4" t="n">
-        <v>0.005861401058731467</v>
+        <v>0.008309297845406316</v>
       </c>
       <c r="EC4" t="n">
         <v>0</v>
@@ -14612,7 +14612,7 @@
         <v>0</v>
       </c>
       <c r="EX4" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY4" t="n">
         <v>0</v>
@@ -14621,13 +14621,13 @@
         <v>0</v>
       </c>
       <c r="FA4" t="n">
-        <v>31.31172703820987</v>
+        <v>32.20646951438269</v>
       </c>
       <c r="FB4" t="n">
-        <v>0.338927913791387</v>
+        <v>0.4777504782706036</v>
       </c>
       <c r="FC4" t="n">
-        <v>0.07174037415993204</v>
+        <v>0.07226864719535553</v>
       </c>
       <c r="FD4" t="n">
         <v>0</v>
@@ -14636,7 +14636,7 @@
         <v>0</v>
       </c>
       <c r="FF4" t="n">
-        <v>17.30365112364506</v>
+        <v>17.80860408288861</v>
       </c>
       <c r="FG4" t="n">
         <v>0</v>
@@ -14830,16 +14830,16 @@
         <v>0.07576910313385271</v>
       </c>
       <c r="AN5" t="n">
-        <v>12.60825199473375</v>
+        <v>52.53864100310895</v>
       </c>
       <c r="AO5" t="n">
-        <v>8.046637077697969</v>
+        <v>37.30420949220779</v>
       </c>
       <c r="AP5" t="n">
         <v>0</v>
       </c>
       <c r="AQ5" t="n">
-        <v>4.561614917035778</v>
+        <v>15.23443151090117</v>
       </c>
       <c r="AR5" t="n">
         <v>0</v>
@@ -14848,19 +14848,19 @@
         <v>0</v>
       </c>
       <c r="AT5" t="n">
-        <v>74.02453503439295</v>
+        <v>121.8121045053803</v>
       </c>
       <c r="AU5" t="n">
-        <v>22.99206310585224</v>
+        <v>69.21498657186895</v>
       </c>
       <c r="AV5" t="n">
-        <v>0.1982666100919121</v>
+        <v>0.2794752628572355</v>
       </c>
       <c r="AW5" t="n">
-        <v>50.8342053184488</v>
+        <v>52.31764267065415</v>
       </c>
       <c r="AX5" t="n">
-        <v>7.105427357601002e-15</v>
+        <v>-1.4210854715202e-14</v>
       </c>
       <c r="AY5" t="n">
         <v>0</v>
@@ -15097,16 +15097,16 @@
         <v>0</v>
       </c>
       <c r="DY5" t="n">
-        <v>0.02275263721155219</v>
+        <v>0.105481226112756</v>
       </c>
       <c r="DZ5" t="n">
-        <v>0.007463787951843422</v>
+        <v>0.0346021209447461</v>
       </c>
       <c r="EA5" t="n">
         <v>0</v>
       </c>
       <c r="EB5" t="n">
-        <v>0.005033787163323094</v>
+        <v>0.007136047578270794</v>
       </c>
       <c r="EC5" t="n">
         <v>0</v>
@@ -15172,7 +15172,7 @@
         <v>0</v>
       </c>
       <c r="EX5" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY5" t="n">
         <v>0</v>
@@ -15181,13 +15181,13 @@
         <v>0</v>
       </c>
       <c r="FA5" t="n">
-        <v>31.97965694956584</v>
+        <v>32.90304280249227</v>
       </c>
       <c r="FB5" t="n">
-        <v>0.1982666100919121</v>
+        <v>0.2794752628572355</v>
       </c>
       <c r="FC5" t="n">
-        <v>0.06519719831077456</v>
+        <v>0.06575874043806755</v>
       </c>
       <c r="FD5" t="n">
         <v>0</v>
@@ -15196,7 +15196,7 @@
         <v>0</v>
       </c>
       <c r="FF5" t="n">
-        <v>18.48643221991453</v>
+        <v>19.02590094756042</v>
       </c>
       <c r="FG5" t="n">
         <v>0</v>
@@ -15390,16 +15390,16 @@
         <v>0.04017522617492097</v>
       </c>
       <c r="AN6" t="n">
-        <v>11.66083194546483</v>
+        <v>47.98375005106177</v>
       </c>
       <c r="AO6" t="n">
-        <v>8.285566716434916</v>
+        <v>38.41188729739226</v>
       </c>
       <c r="AP6" t="n">
         <v>0</v>
       </c>
       <c r="AQ6" t="n">
-        <v>3.375265229029914</v>
+        <v>9.57186275366951</v>
       </c>
       <c r="AR6" t="n">
         <v>0</v>
@@ -15408,16 +15408,16 @@
         <v>0</v>
       </c>
       <c r="AT6" t="n">
-        <v>62.96274096146484</v>
+        <v>109.3780958480188</v>
       </c>
       <c r="AU6" t="n">
-        <v>18.2484411373995</v>
+        <v>63.22885124936731</v>
       </c>
       <c r="AV6" t="n">
-        <v>0.3419922752653987</v>
+        <v>0.4820699813278353</v>
       </c>
       <c r="AW6" t="n">
-        <v>44.37230754879994</v>
+        <v>45.66717461732365</v>
       </c>
       <c r="AX6" t="n">
         <v>0</v>
@@ -15657,16 +15657,16 @@
         <v>0</v>
       </c>
       <c r="DY6" t="n">
-        <v>0.02342823365473416</v>
+        <v>0.1086132912233476</v>
       </c>
       <c r="DZ6" t="n">
-        <v>0.004075053181495331</v>
+        <v>0.01889194654941236</v>
       </c>
       <c r="EA6" t="n">
         <v>0</v>
       </c>
       <c r="EB6" t="n">
-        <v>0.005172248815846901</v>
+        <v>0.007332334967490409</v>
       </c>
       <c r="EC6" t="n">
         <v>0</v>
@@ -15732,7 +15732,7 @@
         <v>0</v>
       </c>
       <c r="EX6" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY6" t="n">
         <v>0</v>
@@ -15741,13 +15741,13 @@
         <v>0</v>
       </c>
       <c r="FA6" t="n">
-        <v>24.73174899418314</v>
+        <v>25.43068093247103</v>
       </c>
       <c r="FB6" t="n">
-        <v>0.3419922752653987</v>
+        <v>0.4820699813278353</v>
       </c>
       <c r="FC6" t="n">
-        <v>0.1035936374226998</v>
+        <v>0.1039599510111723</v>
       </c>
       <c r="FD6" t="n">
         <v>0</v>
@@ -15756,7 +15756,7 @@
         <v>0</v>
       </c>
       <c r="FF6" t="n">
-        <v>18.84771088906654</v>
+        <v>19.3977224051561</v>
       </c>
       <c r="FG6" t="n">
         <v>0</v>
@@ -15950,16 +15950,16 @@
         <v>0.06685252436575988</v>
       </c>
       <c r="AN7" t="n">
-        <v>12.16030209936665</v>
+        <v>48.99286447743441</v>
       </c>
       <c r="AO7" t="n">
-        <v>7.597101077101502</v>
+        <v>35.22016059344256</v>
       </c>
       <c r="AP7" t="n">
         <v>0</v>
       </c>
       <c r="AQ7" t="n">
-        <v>4.56320102226515</v>
+        <v>13.77270388399185</v>
       </c>
       <c r="AR7" t="n">
         <v>0</v>
@@ -15968,19 +15968,19 @@
         <v>0</v>
       </c>
       <c r="AT7" t="n">
-        <v>62.2493383636166</v>
+        <v>109.2717074201711</v>
       </c>
       <c r="AU7" t="n">
-        <v>20.8548915018816</v>
+        <v>66.51489193307084</v>
       </c>
       <c r="AV7" t="n">
-        <v>0.4058793871632823</v>
+        <v>0.5721248190162059</v>
       </c>
       <c r="AW7" t="n">
-        <v>40.98856747457172</v>
+        <v>42.18469066808411</v>
       </c>
       <c r="AX7" t="n">
-        <v>0</v>
+        <v>-7.105427357601002e-15</v>
       </c>
       <c r="AY7" t="n">
         <v>0</v>
@@ -16217,16 +16217,16 @@
         <v>0</v>
       </c>
       <c r="DY7" t="n">
-        <v>0.02148153110395206</v>
+        <v>0.09958837819792177</v>
       </c>
       <c r="DZ7" t="n">
-        <v>0.006217537987600159</v>
+        <v>0.02882450611051433</v>
       </c>
       <c r="EA7" t="n">
         <v>0</v>
       </c>
       <c r="EB7" t="n">
-        <v>0.006284382621345458</v>
+        <v>0.008908929188093469</v>
       </c>
       <c r="EC7" t="n">
         <v>0</v>
@@ -16292,7 +16292,7 @@
         <v>0</v>
       </c>
       <c r="EX7" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY7" t="n">
         <v>0</v>
@@ -16301,13 +16301,13 @@
         <v>0</v>
       </c>
       <c r="FA7" t="n">
-        <v>20.17327539089239</v>
+        <v>20.72935413002364</v>
       </c>
       <c r="FB7" t="n">
-        <v>0.4058793871632823</v>
+        <v>0.5721248190162059</v>
       </c>
       <c r="FC7" t="n">
-        <v>0.05869951665293795</v>
+        <v>0.05929409655469964</v>
       </c>
       <c r="FD7" t="n">
         <v>0</v>
@@ -16316,7 +16316,7 @@
         <v>0</v>
       </c>
       <c r="FF7" t="n">
-        <v>19.92535482212201</v>
+        <v>20.50681400721038</v>
       </c>
       <c r="FG7" t="n">
         <v>0</v>
@@ -16510,16 +16510,16 @@
         <v>0.06137359736084536</v>
       </c>
       <c r="AN8" t="n">
-        <v>13.34287344983246</v>
+        <v>55.34147991565375</v>
       </c>
       <c r="AO8" t="n">
-        <v>8.882346439177008</v>
+        <v>41.17855809202459</v>
       </c>
       <c r="AP8" t="n">
         <v>0</v>
       </c>
       <c r="AQ8" t="n">
-        <v>4.460527010655454</v>
+        <v>14.16292182362916</v>
       </c>
       <c r="AR8" t="n">
         <v>0</v>
@@ -16528,19 +16528,19 @@
         <v>0</v>
       </c>
       <c r="AT8" t="n">
-        <v>67.8433678359375</v>
+        <v>115.8178025890695</v>
       </c>
       <c r="AU8" t="n">
-        <v>24.46354123910693</v>
+        <v>71.06755766119238</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.2747387167451594</v>
+        <v>0.3872698234151387</v>
       </c>
       <c r="AW8" t="n">
-        <v>43.10508788008541</v>
+        <v>44.36297510446196</v>
       </c>
       <c r="AX8" t="n">
-        <v>0</v>
+        <v>-1.4210854715202e-14</v>
       </c>
       <c r="AY8" t="n">
         <v>0</v>
@@ -16777,16 +16777,16 @@
         <v>0</v>
       </c>
       <c r="DY8" t="n">
-        <v>0.02511568549276911</v>
+        <v>0.1164363179444776</v>
       </c>
       <c r="DZ8" t="n">
-        <v>0.006673628384421504</v>
+        <v>0.03093894119017809</v>
       </c>
       <c r="EA8" t="n">
         <v>0</v>
       </c>
       <c r="EB8" t="n">
-        <v>0.005546993562579741</v>
+        <v>0.007863584354011391</v>
       </c>
       <c r="EC8" t="n">
         <v>0</v>
@@ -16852,7 +16852,7 @@
         <v>0</v>
       </c>
       <c r="EX8" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY8" t="n">
         <v>0</v>
@@ -16861,13 +16861,13 @@
         <v>0</v>
       </c>
       <c r="FA8" t="n">
-        <v>29.49369220214028</v>
+        <v>30.31368469163715</v>
       </c>
       <c r="FB8" t="n">
-        <v>0.2747387167451594</v>
+        <v>0.3872698234151387</v>
       </c>
       <c r="FC8" t="n">
-        <v>0.09726974309297991</v>
+        <v>0.09766821082590436</v>
       </c>
       <c r="FD8" t="n">
         <v>0</v>
@@ -16876,7 +16876,7 @@
         <v>0</v>
       </c>
       <c r="FF8" t="n">
-        <v>13.49435992054572</v>
+        <v>13.88815062554126</v>
       </c>
       <c r="FG8" t="n">
         <v>0</v>
@@ -17070,16 +17070,16 @@
         <v>0.03149019993453546</v>
       </c>
       <c r="AN9" t="n">
-        <v>11.80149927366452</v>
+        <v>47.48509678100757</v>
       </c>
       <c r="AO9" t="n">
-        <v>8.377300894103382</v>
+        <v>38.83716694506329</v>
       </c>
       <c r="AP9" t="n">
         <v>0</v>
       </c>
       <c r="AQ9" t="n">
-        <v>3.424198379561138</v>
+        <v>8.64792983594428</v>
       </c>
       <c r="AR9" t="n">
         <v>0</v>
@@ -17088,19 +17088,19 @@
         <v>0</v>
       </c>
       <c r="AT9" t="n">
-        <v>61.59357552985915</v>
+        <v>107.867153854678</v>
       </c>
       <c r="AU9" t="n">
-        <v>17.62779247367044</v>
+        <v>62.47247001385377</v>
       </c>
       <c r="AV9" t="n">
-        <v>0.3835239835955752</v>
+        <v>0.5406127944475297</v>
       </c>
       <c r="AW9" t="n">
-        <v>43.58225907259314</v>
+        <v>44.85407104637666</v>
       </c>
       <c r="AX9" t="n">
-        <v>-7.105427357601002e-15</v>
+        <v>0</v>
       </c>
       <c r="AY9" t="n">
         <v>0</v>
@@ -17337,16 +17337,16 @@
         <v>0</v>
       </c>
       <c r="DY9" t="n">
-        <v>0.0236876208303004</v>
+        <v>0.1098158101692727</v>
       </c>
       <c r="DZ9" t="n">
-        <v>0.003229477509946293</v>
+        <v>0.01497185773611101</v>
       </c>
       <c r="EA9" t="n">
         <v>0</v>
       </c>
       <c r="EB9" t="n">
-        <v>0.00615188791350888</v>
+        <v>0.008721100718530854</v>
       </c>
       <c r="EC9" t="n">
         <v>0</v>
@@ -17412,7 +17412,7 @@
         <v>0</v>
       </c>
       <c r="EX9" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY9" t="n">
         <v>0</v>
@@ -17421,13 +17421,13 @@
         <v>0</v>
       </c>
       <c r="FA9" t="n">
-        <v>22.67909698300534</v>
+        <v>23.27151744402144</v>
       </c>
       <c r="FB9" t="n">
-        <v>0.3835239835955752</v>
+        <v>0.5406127944475297</v>
       </c>
       <c r="FC9" t="n">
-        <v>0.04986302666280219</v>
+        <v>0.05050253612232956</v>
       </c>
       <c r="FD9" t="n">
         <v>0</v>
@@ -17436,7 +17436,7 @@
         <v>0</v>
       </c>
       <c r="FF9" t="n">
-        <v>18.85710077491159</v>
+        <v>19.40738630546264</v>
       </c>
       <c r="FG9" t="n">
         <v>0</v>
@@ -17630,16 +17630,16 @@
         <v>0.02252933372593857</v>
       </c>
       <c r="AN10" t="n">
-        <v>12.09269637468582</v>
+        <v>49.3886957956508</v>
       </c>
       <c r="AO10" t="n">
-        <v>9.102896983728815</v>
+        <v>42.20103041656679</v>
       </c>
       <c r="AP10" t="n">
         <v>0</v>
       </c>
       <c r="AQ10" t="n">
-        <v>2.989799390957009</v>
+        <v>7.187665379084021</v>
       </c>
       <c r="AR10" t="n">
         <v>0</v>
@@ -17648,16 +17648,16 @@
         <v>0</v>
       </c>
       <c r="AT10" t="n">
-        <v>67.26908818467135</v>
+        <v>114.6062087949535</v>
       </c>
       <c r="AU10" t="n">
-        <v>21.51077123520369</v>
+        <v>67.33756740460419</v>
       </c>
       <c r="AV10" t="n">
-        <v>0.4600573509409428</v>
+        <v>0.6484937076596962</v>
       </c>
       <c r="AW10" t="n">
-        <v>45.2982595985267</v>
+        <v>46.62014768268961</v>
       </c>
       <c r="AX10" t="n">
         <v>0</v>
@@ -17897,16 +17897,16 @@
         <v>0</v>
       </c>
       <c r="DY10" t="n">
-        <v>0.02573931328641045</v>
+        <v>0.1193274563957989</v>
       </c>
       <c r="DZ10" t="n">
-        <v>0.002510618403415571</v>
+        <v>0.01163922691823459</v>
       </c>
       <c r="EA10" t="n">
         <v>0</v>
       </c>
       <c r="EB10" t="n">
-        <v>0.005680612804685824</v>
+        <v>0.008053006997064105</v>
       </c>
       <c r="EC10" t="n">
         <v>0</v>
@@ -17972,7 +17972,7 @@
         <v>0</v>
       </c>
       <c r="EX10" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY10" t="n">
         <v>0</v>
@@ -17981,13 +17981,13 @@
         <v>0</v>
       </c>
       <c r="FA10" t="n">
-        <v>26.97487633157158</v>
+        <v>27.74938270756887</v>
       </c>
       <c r="FB10" t="n">
-        <v>0.4600573509409428</v>
+        <v>0.6484937076596962</v>
       </c>
       <c r="FC10" t="n">
-        <v>0.0700469943332037</v>
+        <v>0.07058387743968812</v>
       </c>
       <c r="FD10" t="n">
         <v>0</v>
@@ -17996,7 +17996,7 @@
         <v>0</v>
       </c>
       <c r="FF10" t="n">
-        <v>17.48181575678515</v>
+        <v>17.99196789382613</v>
       </c>
       <c r="FG10" t="n">
         <v>0</v>
@@ -18190,16 +18190,16 @@
         <v>0.07339068507189184</v>
       </c>
       <c r="AN11" t="n">
-        <v>12.38702631841619</v>
+        <v>51.0206227831736</v>
       </c>
       <c r="AO11" t="n">
-        <v>7.829223284939238</v>
+        <v>36.29627914897833</v>
       </c>
       <c r="AP11" t="n">
         <v>0</v>
       </c>
       <c r="AQ11" t="n">
-        <v>4.557803033476947</v>
+        <v>14.72434363419528</v>
       </c>
       <c r="AR11" t="n">
         <v>0</v>
@@ -18208,16 +18208,16 @@
         <v>0</v>
       </c>
       <c r="AT11" t="n">
-        <v>67.52694017561984</v>
+        <v>114.2573010594789</v>
       </c>
       <c r="AU11" t="n">
-        <v>19.19652646658173</v>
+        <v>64.42943188051099</v>
       </c>
       <c r="AV11" t="n">
-        <v>0.2289191849632906</v>
+        <v>0.3226829235695374</v>
       </c>
       <c r="AW11" t="n">
-        <v>48.10149452407482</v>
+        <v>49.50518625539842</v>
       </c>
       <c r="AX11" t="n">
         <v>0</v>
@@ -18457,16 +18457,16 @@
         <v>0</v>
       </c>
       <c r="DY11" t="n">
-        <v>0.02213787888410913</v>
+        <v>0.1026312065067299</v>
       </c>
       <c r="DZ11" t="n">
-        <v>0.007034161780892995</v>
+        <v>0.03261037401621993</v>
       </c>
       <c r="EA11" t="n">
         <v>0</v>
       </c>
       <c r="EB11" t="n">
-        <v>0.005452969817673984</v>
+        <v>0.007730293474726031</v>
       </c>
       <c r="EC11" t="n">
         <v>0</v>
@@ -18532,7 +18532,7 @@
         <v>0</v>
       </c>
       <c r="EX11" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY11" t="n">
         <v>0</v>
@@ -18541,13 +18541,13 @@
         <v>0</v>
       </c>
       <c r="FA11" t="n">
-        <v>28.09338064850041</v>
+        <v>28.9125600674706</v>
       </c>
       <c r="FB11" t="n">
-        <v>0.2289191849632906</v>
+        <v>0.3226829235695374</v>
       </c>
       <c r="FC11" t="n">
-        <v>0.07764037666585852</v>
+        <v>0.07813865085516734</v>
       </c>
       <c r="FD11" t="n">
         <v>0</v>
@@ -18556,7 +18556,7 @@
         <v>0</v>
       </c>
       <c r="FF11" t="n">
-        <v>19.37920407279947</v>
+        <v>19.94472555577557</v>
       </c>
       <c r="FG11" t="n">
         <v>0</v>
@@ -18750,16 +18750,16 @@
         <v>0.04752246555633087</v>
       </c>
       <c r="AN12" t="n">
-        <v>13.65199649143812</v>
+        <v>55.50886057679018</v>
       </c>
       <c r="AO12" t="n">
-        <v>9.266384181354702</v>
+        <v>42.95895706476045</v>
       </c>
       <c r="AP12" t="n">
         <v>0</v>
       </c>
       <c r="AQ12" t="n">
-        <v>4.385612310083412</v>
+        <v>12.54990351202973</v>
       </c>
       <c r="AR12" t="n">
         <v>0</v>
@@ -18768,16 +18768,16 @@
         <v>0</v>
       </c>
       <c r="AT12" t="n">
-        <v>71.04559050229864</v>
+        <v>118.7417710419446</v>
       </c>
       <c r="AU12" t="n">
-        <v>22.66395127102196</v>
+        <v>68.78244388123038</v>
       </c>
       <c r="AV12" t="n">
-        <v>0.4358993665413336</v>
+        <v>0.6144407774307891</v>
       </c>
       <c r="AW12" t="n">
-        <v>47.94573986473534</v>
+        <v>49.34488638328347</v>
       </c>
       <c r="AX12" t="n">
         <v>0</v>
@@ -19017,16 +19017,16 @@
         <v>0</v>
       </c>
       <c r="DY12" t="n">
-        <v>0.02620158899990387</v>
+        <v>0.1214705666035543</v>
       </c>
       <c r="DZ12" t="n">
-        <v>0.00539090896868146</v>
+        <v>0.02499225397880725</v>
       </c>
       <c r="EA12" t="n">
         <v>0</v>
       </c>
       <c r="EB12" t="n">
-        <v>0.006624467223327889</v>
+        <v>0.009391043314424906</v>
       </c>
       <c r="EC12" t="n">
         <v>0</v>
@@ -19092,7 +19092,7 @@
         <v>0</v>
       </c>
       <c r="EX12" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY12" t="n">
         <v>0</v>
@@ -19101,13 +19101,13 @@
         <v>0</v>
       </c>
       <c r="FA12" t="n">
-        <v>19.11408142922745</v>
+        <v>19.63207659202659</v>
       </c>
       <c r="FB12" t="n">
-        <v>0.4358993665413336</v>
+        <v>0.6144407774307891</v>
       </c>
       <c r="FC12" t="n">
-        <v>0.08293501192051581</v>
+        <v>0.08340636528257446</v>
       </c>
       <c r="FD12" t="n">
         <v>0</v>
@@ -19116,7 +19116,7 @@
         <v>0</v>
       </c>
       <c r="FF12" t="n">
-        <v>27.64520019771121</v>
+        <v>28.45193893446481</v>
       </c>
       <c r="FG12" t="n">
         <v>0</v>
@@ -19310,16 +19310,16 @@
         <v>0.03797966659950064</v>
       </c>
       <c r="AN13" t="n">
-        <v>11.25528640141068</v>
+        <v>43.63141255631781</v>
       </c>
       <c r="AO13" t="n">
-        <v>7.35163815351133</v>
+        <v>34.08219447967856</v>
       </c>
       <c r="AP13" t="n">
         <v>0</v>
       </c>
       <c r="AQ13" t="n">
-        <v>3.903648247899352</v>
+        <v>9.54921807663926</v>
       </c>
       <c r="AR13" t="n">
         <v>0</v>
@@ -19328,19 +19328,19 @@
         <v>0</v>
       </c>
       <c r="AT13" t="n">
-        <v>66.74067914458918</v>
+        <v>113.6179928257156</v>
       </c>
       <c r="AU13" t="n">
-        <v>19.73954867922693</v>
+        <v>65.11982459969822</v>
       </c>
       <c r="AV13" t="n">
-        <v>0.3297922791184394</v>
+        <v>0.4648729498738348</v>
       </c>
       <c r="AW13" t="n">
-        <v>46.67133818624382</v>
+        <v>48.03329527614358</v>
       </c>
       <c r="AX13" t="n">
-        <v>0</v>
+        <v>-7.105427357601002e-15</v>
       </c>
       <c r="AY13" t="n">
         <v>0</v>
@@ -19577,16 +19577,16 @@
         <v>0</v>
       </c>
       <c r="DY13" t="n">
-        <v>0.0207874611719536</v>
+        <v>0.09637066999317691</v>
       </c>
       <c r="DZ13" t="n">
-        <v>0.003418125488835482</v>
+        <v>0.01584642976624129</v>
       </c>
       <c r="EA13" t="n">
         <v>0</v>
       </c>
       <c r="EB13" t="n">
-        <v>0.007276801217738087</v>
+        <v>0.01031581153961969</v>
       </c>
       <c r="EC13" t="n">
         <v>0</v>
@@ -19652,7 +19652,7 @@
         <v>0</v>
       </c>
       <c r="EX13" t="n">
-        <v>12.770179125</v>
+        <v>56.44040149761619</v>
       </c>
       <c r="EY13" t="n">
         <v>0</v>
@@ -19661,13 +19661,13 @@
         <v>0</v>
       </c>
       <c r="FA13" t="n">
-        <v>17.63021422162677</v>
+        <v>18.14141907977346</v>
       </c>
       <c r="FB13" t="n">
-        <v>0.3297922791184394</v>
+        <v>0.4648729498738348</v>
       </c>
       <c r="FC13" t="n">
-        <v>0.08982424459972932</v>
+        <v>0.09026056932734516</v>
       </c>
       <c r="FD13" t="n">
         <v>0</v>
@@ -19676,7 +19676,7 @@
         <v>0</v>
       </c>
       <c r="FF13" t="n">
-        <v>27.80740016731077</v>
+        <v>28.61887220306892</v>
       </c>
       <c r="FG13" t="n">
         <v>0</v>

</xml_diff>